<commit_message>
Publish Base profiles v2.0.0-rc2
</commit_message>
<xml_diff>
--- a/fhir/finnish-base-profiles/CodeSystem-fi-base-security-label-cs.xlsx
+++ b/fhir/finnish-base-profiles/CodeSystem-fi-base-security-label-cs.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.0-rc1</t>
+    <t>2.0.0-rc2</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-02-06T19:06:41+02:00</t>
+    <t>2025-05-11T16:31:48+03:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Roll back base v2.0.0-rc2
It was published with an old version of the publisher. Let's update.
</commit_message>
<xml_diff>
--- a/fhir/finnish-base-profiles/CodeSystem-fi-base-security-label-cs.xlsx
+++ b/fhir/finnish-base-profiles/CodeSystem-fi-base-security-label-cs.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.0-rc2</t>
+    <t>2.0.0-rc1</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-11T16:31:48+03:00</t>
+    <t>2025-02-06T19:06:41+02:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Republish Base Profiles v2.0.0-rc2
Now published with the latest version of the IG publisher
</commit_message>
<xml_diff>
--- a/fhir/finnish-base-profiles/CodeSystem-fi-base-security-label-cs.xlsx
+++ b/fhir/finnish-base-profiles/CodeSystem-fi-base-security-label-cs.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.0-rc1</t>
+    <t>2.0.0-rc2</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-02-06T19:06:41+02:00</t>
+    <t>2025-05-11T20:18:22+03:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>